<commit_message>
Check rank deficiency. ct --> mu.
</commit_message>
<xml_diff>
--- a/vignettes/_figures/mcp_glm_status.xlsx
+++ b/vignettes/_figures/mcp_glm_status.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t xml:space="preserve">Link</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t xml:space="preserve">Exponential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative binomial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beta</t>
   </si>
   <si>
     <t xml:space="preserve">identity</t>
@@ -302,21 +308,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N27" activeCellId="0" sqref="N27"/>
+      <selection pane="topLeft" activeCell="N29" activeCellId="0" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,27 +363,33 @@
       <c r="H2" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -383,148 +397,148 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>